<commit_message>
specs v3: specs added
</commit_message>
<xml_diff>
--- a/v3/Specs_v3.xlsx
+++ b/v3/Specs_v3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victoriadudley\Desktop\Team-Infinite\v3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.bulley\Team-Infinite\v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>If both distances are the same, output first ID</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>VERSION3</t>
+  </si>
+  <si>
+    <t>Add exchange button</t>
+  </si>
+  <si>
+    <t>Remove exchange2 row</t>
+  </si>
+  <si>
+    <t>Add dropdown and populate with added exchanges</t>
+  </si>
+  <si>
+    <t>(reset button)</t>
+  </si>
+  <si>
+    <t>(placeholder text)</t>
   </si>
 </sst>
 </file>
@@ -413,7 +428,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
@@ -462,6 +477,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -744,24 +761,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="73.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="73.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="67.44140625" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="67.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -777,7 +794,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="30" t="s">
@@ -787,7 +804,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -795,7 +812,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="23" t="s">
         <v>17</v>
@@ -811,7 +828,7 @@
       </c>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="12" t="s">
         <v>30</v>
@@ -821,7 +838,7 @@
       <c r="E5" s="10"/>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="21" t="s">
         <v>3</v>
@@ -837,7 +854,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="22" t="s">
         <v>5</v>
@@ -853,7 +870,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="21" t="s">
         <v>2</v>
@@ -869,7 +886,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="22" t="s">
         <v>1</v>
@@ -885,7 +902,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="21" t="s">
         <v>1</v>
@@ -901,7 +918,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="22" t="s">
         <v>4</v>
@@ -917,7 +934,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="21" t="s">
         <v>7</v>
@@ -933,7 +950,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="22" t="s">
         <v>7</v>
@@ -949,7 +966,7 @@
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="13" t="s">
         <v>31</v>
@@ -959,7 +976,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="20" t="s">
         <v>15</v>
@@ -975,7 +992,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="20"/>
       <c r="C16" s="9" t="s">
@@ -985,7 +1002,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="14" t="s">
         <v>18</v>
@@ -1001,7 +1018,7 @@
       </c>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="13" t="s">
         <v>32</v>
@@ -1011,7 +1028,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="20" t="s">
         <v>21</v>
@@ -1029,68 +1046,73 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="33"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="33"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="33"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="33"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="33"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D25" s="27">
         <f>SUM(D6:D19)</f>
         <v>4</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E25" s="28">
         <f>SUM(E6:E19)</f>
         <v>5.5</v>
       </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="29">
-        <f>SUM(D20+E20)</f>
-        <v>9.5</v>
-      </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1098,7 +1120,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1106,15 +1128,20 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="29">
+        <f>SUM(D25+E25)</f>
+        <v>9.5</v>
+      </c>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1122,7 +1149,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1130,7 +1157,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1138,7 +1165,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1146,7 +1173,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1154,7 +1181,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1162,7 +1189,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1170,7 +1197,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1178,7 +1205,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1186,6 +1213,46 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>